<commit_message>
Finished projections of econ result ANSES 10/12/2019 legislation
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Prospective_extrapolated_results/Projections_2014_q4_start/Late_2019_legislation/total_retirement_pensions.xlsx
+++ b/Excel_files_for_MISSAR/Prospective_extrapolated_results/Projections_2014_q4_start/Late_2019_legislation/total_retirement_pensions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Low scenario_2" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,6 +48,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Use total net pensions, post-2016 from period2 167 (third quarter of 2016) onwards.</t>
         </r>
@@ -83,6 +84,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Use total net pensions, post-2016 from period2 167 (third quarter of 2016) onwards.</t>
         </r>
@@ -99,10 +101,30 @@
   </authors>
   <commentList>
     <comment ref="F2" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+      </text>
     </comment>
     <comment ref="G2" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+      </text>
     </comment>
   </commentList>
 </comments>
@@ -274,7 +296,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -310,11 +332,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -621,7 +638,7 @@
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5384,11 +5401,11 @@
   </sheetPr>
   <dimension ref="A1:AD120"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="17" width="14.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.95"/>
@@ -5399,7 +5416,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.48"/>
   </cols>
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14288,7 +14305,7 @@
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="16.01"/>
   </cols>
@@ -22696,11 +22713,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N19" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N19" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Z40" activeCellId="0" sqref="Z40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="17" width="14.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.46"/>
@@ -31107,5 +31124,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>